<commit_message>
More tests added (merged from github repo).
Fixed tests

Change-Id: I4b804c742d7446d2daa7243ee6f5770fd02aae0c
</commit_message>
<xml_diff>
--- a/vaadin-spreadsheet-flow-parent/spreadsheet-charts-integration/src/test/resources/test_sheets/StyleSample - Background and Border.xlsx
+++ b/vaadin-spreadsheet-flow-parent/spreadsheet-charts-integration/src/test/resources/test_sheets/StyleSample - Background and Border.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="2240" yWindow="5120" windowWidth="34220" windowHeight="15460" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Taul1" sheetId="1" r:id="rId1"/>
@@ -183,11 +183,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1979665248"/>
-        <c:axId val="-2052694432"/>
+        <c:axId val="-2078889824"/>
+        <c:axId val="-2059144080"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1979665248"/>
+        <c:axId val="-2078889824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -229,7 +229,7 @@
             <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2052694432"/>
+        <c:crossAx val="-2059144080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -237,7 +237,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2052694432"/>
+        <c:axId val="-2059144080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -288,7 +288,7 @@
             <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1979665248"/>
+        <c:crossAx val="-2078889824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -436,11 +436,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1831590688"/>
-        <c:axId val="-2011848592"/>
+        <c:axId val="-2119038704"/>
+        <c:axId val="-2019420784"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1831590688"/>
+        <c:axId val="-2119038704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -482,7 +482,7 @@
             <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2011848592"/>
+        <c:crossAx val="-2019420784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -490,7 +490,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2011848592"/>
+        <c:axId val="-2019420784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -541,7 +541,7 @@
             <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1831590688"/>
+        <c:crossAx val="-2119038704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -722,11 +722,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1831391856"/>
-        <c:axId val="1831670736"/>
+        <c:axId val="-2019392304"/>
+        <c:axId val="-2019389104"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1831391856"/>
+        <c:axId val="-2019392304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -768,7 +768,7 @@
             <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1831670736"/>
+        <c:crossAx val="-2019389104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -776,7 +776,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1831670736"/>
+        <c:axId val="-2019389104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -827,7 +827,7 @@
             <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1831391856"/>
+        <c:crossAx val="-2019392304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -998,11 +998,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2011942272"/>
-        <c:axId val="1835772368"/>
+        <c:axId val="-2019361472"/>
+        <c:axId val="-2019358272"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2011942272"/>
+        <c:axId val="-2019361472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1044,7 +1044,7 @@
             <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1835772368"/>
+        <c:crossAx val="-2019358272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1052,7 +1052,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1835772368"/>
+        <c:axId val="-2019358272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1103,7 +1103,7 @@
             <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2011942272"/>
+        <c:crossAx val="-2019361472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1278,11 +1278,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1835100032"/>
-        <c:axId val="1835902768"/>
+        <c:axId val="-2019330752"/>
+        <c:axId val="-2019327552"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1835100032"/>
+        <c:axId val="-2019330752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1324,7 +1324,7 @@
             <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1835902768"/>
+        <c:crossAx val="-2019327552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1332,7 +1332,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1835902768"/>
+        <c:axId val="-2019327552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1383,7 +1383,7 @@
             <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1835100032"/>
+        <c:crossAx val="-2019330752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1554,11 +1554,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2011934720"/>
-        <c:axId val="1835094336"/>
+        <c:axId val="-2019299888"/>
+        <c:axId val="-2019296688"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2011934720"/>
+        <c:axId val="-2019299888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1600,7 +1600,7 @@
             <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1835094336"/>
+        <c:crossAx val="-2019296688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1608,7 +1608,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1835094336"/>
+        <c:axId val="-2019296688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1659,7 +1659,7 @@
             <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2011934720"/>
+        <c:crossAx val="-2019299888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1831,11 +1831,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2052641424"/>
-        <c:axId val="1835589936"/>
+        <c:axId val="-2019271488"/>
+        <c:axId val="-2019268288"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2052641424"/>
+        <c:axId val="-2019271488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1877,7 +1877,7 @@
             <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1835589936"/>
+        <c:crossAx val="-2019268288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1885,7 +1885,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1835589936"/>
+        <c:axId val="-2019268288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1936,7 +1936,7 @@
             <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2052641424"/>
+        <c:crossAx val="-2019271488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2108,11 +2108,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1849073712"/>
-        <c:axId val="-2016874336"/>
+        <c:axId val="-2019240784"/>
+        <c:axId val="-2019237584"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1849073712"/>
+        <c:axId val="-2019240784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2154,7 +2154,7 @@
             <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2016874336"/>
+        <c:crossAx val="-2019237584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2162,7 +2162,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2016874336"/>
+        <c:axId val="-2019237584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2213,7 +2213,7 @@
             <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1849073712"/>
+        <c:crossAx val="-2019240784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2384,11 +2384,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1985053936"/>
-        <c:axId val="-1981369504"/>
+        <c:axId val="-2019209824"/>
+        <c:axId val="-2019206624"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1985053936"/>
+        <c:axId val="-2019209824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2430,7 +2430,7 @@
             <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1981369504"/>
+        <c:crossAx val="-2019206624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2438,7 +2438,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1981369504"/>
+        <c:axId val="-2019206624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2489,7 +2489,7 @@
             <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1985053936"/>
+        <c:crossAx val="-2019209824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2656,11 +2656,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1832110512"/>
-        <c:axId val="-1978703584"/>
+        <c:axId val="-2078252992"/>
+        <c:axId val="-2078249792"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1832110512"/>
+        <c:axId val="-2078252992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2702,7 +2702,7 @@
             <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1978703584"/>
+        <c:crossAx val="-2078249792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2710,7 +2710,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1978703584"/>
+        <c:axId val="-2078249792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2761,7 +2761,7 @@
             <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1832110512"/>
+        <c:crossAx val="-2078252992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2848,7 +2848,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="fi-FI"/>
-              <a:t>Kaav4567</a:t>
+              <a:t>Gradient angle 0</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -2932,11 +2932,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1847743504"/>
-        <c:axId val="1847717296"/>
+        <c:axId val="-2078178112"/>
+        <c:axId val="-2078174912"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1847743504"/>
+        <c:axId val="-2078178112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2978,7 +2978,7 @@
             <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1847717296"/>
+        <c:crossAx val="-2078174912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2986,7 +2986,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1847717296"/>
+        <c:axId val="-2078174912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3037,7 +3037,7 @@
             <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1847743504"/>
+        <c:crossAx val="-2078178112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3227,11 +3227,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1981444704"/>
-        <c:axId val="-1980892560"/>
+        <c:axId val="-2059044384"/>
+        <c:axId val="-2059041184"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1981444704"/>
+        <c:axId val="-2059044384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3273,7 +3273,7 @@
             <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1980892560"/>
+        <c:crossAx val="-2059041184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3281,7 +3281,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1980892560"/>
+        <c:axId val="-2059041184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3332,7 +3332,7 @@
             <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1981444704"/>
+        <c:crossAx val="-2059044384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3417,7 +3417,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="fi-FI"/>
-              <a:t>Kaav4567</a:t>
+              <a:t>Gradient angle 60 </a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -3501,11 +3501,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1850909072"/>
-        <c:axId val="1853673088"/>
+        <c:axId val="-2078147008"/>
+        <c:axId val="-2078143808"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1850909072"/>
+        <c:axId val="-2078147008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3547,7 +3547,7 @@
             <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1853673088"/>
+        <c:crossAx val="-2078143808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3555,7 +3555,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1853673088"/>
+        <c:axId val="-2078143808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3606,7 +3606,7 @@
             <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1850909072"/>
+        <c:crossAx val="-2078147008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3712,7 +3712,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="fi-FI"/>
-              <a:t>Kaav4567</a:t>
+              <a:t>Gradient angle 110</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -3796,11 +3796,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1860078224"/>
-        <c:axId val="1861757648"/>
+        <c:axId val="-2078115808"/>
+        <c:axId val="-2078112608"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1860078224"/>
+        <c:axId val="-2078115808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3842,7 +3842,7 @@
             <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1861757648"/>
+        <c:crossAx val="-2078112608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3850,7 +3850,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1861757648"/>
+        <c:axId val="-2078112608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3901,7 +3901,7 @@
             <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1860078224"/>
+        <c:crossAx val="-2078115808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4007,7 +4007,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="fi-FI"/>
-              <a:t>Kaav4567</a:t>
+              <a:t>Gradient angle 260</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -4091,11 +4091,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1860815520"/>
-        <c:axId val="1845625872"/>
+        <c:axId val="-2078084240"/>
+        <c:axId val="-2078081040"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1860815520"/>
+        <c:axId val="-2078084240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4137,7 +4137,7 @@
             <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1845625872"/>
+        <c:crossAx val="-2078081040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4145,7 +4145,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1845625872"/>
+        <c:axId val="-2078081040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4196,7 +4196,7 @@
             <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1860815520"/>
+        <c:crossAx val="-2078084240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4245,6 +4245,560 @@
         </a:schemeClr>
       </a:solidFill>
       <a:prstDash val="dash"/>
+      <a:bevel/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fi-FI"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart23.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="fi-FI"/>
+  <c:roundedCorners val="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fi-FI"/>
+              <a:t>Solid green background</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="fi-FI" baseline="0"/>
+              <a:t> and blue thick frame</a:t>
+            </a:r>
+            <a:endParaRPr lang="fi-FI"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fi-FI"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Taul1!$A$1:$A$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="-2120591168"/>
+        <c:axId val="-2063209472"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2120591168"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fi-FI"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2063209472"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2063209472"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fi-FI"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2120591168"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="accent6"/>
+    </a:solidFill>
+    <a:ln w="28575" cap="rnd" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="accent1">
+          <a:lumMod val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:prstDash val="solid"/>
+      <a:bevel/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fi-FI"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart24.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="fi-FI"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fi-FI"/>
+              <a:t>Brown 70% transparent background and thin green frame</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fi-FI"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Taul1!$A$1:$A$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="-2078464176"/>
+        <c:axId val="-1976832176"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2078464176"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fi-FI"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1976832176"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-1976832176"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fi-FI"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2078464176"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="accent2">
+        <a:lumMod val="75000"/>
+        <a:alpha val="30000"/>
+      </a:schemeClr>
+    </a:solidFill>
+    <a:ln w="6350" cap="rnd" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="accent6">
+          <a:lumMod val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:prstDash val="solid"/>
       <a:bevel/>
     </a:ln>
     <a:effectLst/>
@@ -4386,11 +4940,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1849309888"/>
-        <c:axId val="1831639392"/>
+        <c:axId val="-2118239552"/>
+        <c:axId val="-2118236352"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1849309888"/>
+        <c:axId val="-2118239552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4432,7 +4986,7 @@
             <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1831639392"/>
+        <c:crossAx val="-2118236352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4440,7 +4994,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1831639392"/>
+        <c:axId val="-2118236352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4491,7 +5045,7 @@
             <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1849309888"/>
+        <c:crossAx val="-2118239552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4663,11 +5217,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1831078368"/>
-        <c:axId val="1847478880"/>
+        <c:axId val="-2118205424"/>
+        <c:axId val="-2118202224"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1831078368"/>
+        <c:axId val="-2118205424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4709,7 +5263,7 @@
             <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1847478880"/>
+        <c:crossAx val="-2118202224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4717,7 +5271,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1847478880"/>
+        <c:axId val="-2118202224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4768,7 +5322,7 @@
             <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1831078368"/>
+        <c:crossAx val="-2118205424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4937,11 +5491,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2016578176"/>
-        <c:axId val="1830871792"/>
+        <c:axId val="-2118171392"/>
+        <c:axId val="-2118168192"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2016578176"/>
+        <c:axId val="-2118171392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4983,7 +5537,7 @@
             <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1830871792"/>
+        <c:crossAx val="-2118168192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4991,7 +5545,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1830871792"/>
+        <c:axId val="-2118168192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5042,7 +5596,7 @@
             <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2016578176"/>
+        <c:crossAx val="-2118171392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5213,11 +5767,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1831642752"/>
-        <c:axId val="1847285920"/>
+        <c:axId val="-2118140528"/>
+        <c:axId val="-2119169648"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1831642752"/>
+        <c:axId val="-2118140528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5259,7 +5813,7 @@
             <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1847285920"/>
+        <c:crossAx val="-2119169648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5267,7 +5821,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1847285920"/>
+        <c:axId val="-2119169648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5318,7 +5872,7 @@
             <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1831642752"/>
+        <c:crossAx val="-2118140528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5489,11 +6043,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1846604416"/>
-        <c:axId val="1835713152"/>
+        <c:axId val="-2119144144"/>
+        <c:axId val="-2119140944"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1846604416"/>
+        <c:axId val="-2119144144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5535,7 +6089,7 @@
             <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1835713152"/>
+        <c:crossAx val="-2119140944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5543,7 +6097,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1835713152"/>
+        <c:axId val="-2119140944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5594,7 +6148,7 @@
             <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1846604416"/>
+        <c:crossAx val="-2119144144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5763,11 +6317,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2016546400"/>
-        <c:axId val="-2016648000"/>
+        <c:axId val="-2119113520"/>
+        <c:axId val="-2119110320"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2016546400"/>
+        <c:axId val="-2119113520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5809,7 +6363,7 @@
             <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2016648000"/>
+        <c:crossAx val="-2119110320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5817,7 +6371,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2016648000"/>
+        <c:axId val="-2119110320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5868,7 +6422,7 @@
             <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2016546400"/>
+        <c:crossAx val="-2119113520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6037,11 +6591,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1847059680"/>
-        <c:axId val="1835374976"/>
+        <c:axId val="-2119082336"/>
+        <c:axId val="-2119079136"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1847059680"/>
+        <c:axId val="-2119082336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6083,7 +6637,7 @@
             <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1835374976"/>
+        <c:crossAx val="-2119079136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6091,7 +6645,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1835374976"/>
+        <c:axId val="-2119079136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6142,7 +6696,7 @@
             <a:endParaRPr lang="fi-FI"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1847059680"/>
+        <c:crossAx val="-2119082336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6792,6 +7346,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors23.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors24.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -14115,6 +14749,1012 @@
 </file>
 
 <file path=xl/charts/style22.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style23.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style24.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -18726,16 +20366,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>444500</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>469900</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -18758,16 +20398,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>444500</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>469900</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -18790,16 +20430,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>444500</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>469900</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -18822,16 +20462,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>444500</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>469900</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -18847,6 +20487,70 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>482600</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Kaavio 5"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>482600</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Kaavio 6"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -19177,7 +20881,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="T22" sqref="T22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>